<commit_message>
Registration Test Cases Added
</commit_message>
<xml_diff>
--- a/Test_Case_Design/Registration_Testing_Test_Cases.xlsx
+++ b/Test_Case_Design/Registration_Testing_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wasana\University\Projects\QA-Portfolio\Test_Case_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA111CB2-CEA3-42D2-9A3A-BA87EC97B337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C809FC-B933-4361-AF43-0FACAC118BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>TS-05</t>
   </si>
   <si>
-    <t>Error message should be displayed</t>
-  </si>
-  <si>
     <t>Error message displayed</t>
   </si>
   <si>
@@ -117,76 +114,31 @@
     <t>TS-08</t>
   </si>
   <si>
-    <t>Validation message for email should appear</t>
-  </si>
-  <si>
-    <t>Validation message for email appeared</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
     <t>TS-09</t>
   </si>
   <si>
-    <t>Validation message for password should appear</t>
-  </si>
-  <si>
-    <t>Validation message for password appeared</t>
-  </si>
-  <si>
     <t>TS-10</t>
   </si>
   <si>
-    <t>Validation message appeared</t>
-  </si>
-  <si>
     <t>TS-11</t>
   </si>
   <si>
-    <t>Password should be masked</t>
-  </si>
-  <si>
-    <t>Password masked</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
     <t>TS-12</t>
   </si>
   <si>
-    <t>Password visibility should toggle</t>
-  </si>
-  <si>
-    <t>Password visibility not toggled</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>Mandatory field should be appeared</t>
-  </si>
-  <si>
-    <t>Mandatory field appeared</t>
-  </si>
-  <si>
     <t>TC-11</t>
   </si>
   <si>
-    <t>Verify that error messages are user-friendly, readable, and meaningful.</t>
-  </si>
-  <si>
-    <t>The error messages are user-friendly, readable, and meaningful.</t>
-  </si>
-  <si>
     <t>TC-12</t>
-  </si>
-  <si>
-    <t>Verify that the Login button behavior is correct (enabled/disabled) based on input fields.</t>
-  </si>
-  <si>
-    <t>Login button behavior is incorrect (enabled/disabled) based on input fields.</t>
   </si>
   <si>
     <t>Verify registration with valid user details</t>
@@ -321,6 +273,44 @@
   </si>
   <si>
     <t xml:space="preserve">First Name: Wasana                                                         Last Name: Weerakon                                                    Email:  wasa@gmail.com                                                                                Password:                                                                 Confirm Password: wasana123                                                      </t>
+  </si>
+  <si>
+    <t>Validation messages are displayed for all mandatory fields</t>
+  </si>
+  <si>
+    <t>System shows email format error
+Valid email accepted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error displayed indicating passwords do not match	</t>
+  </si>
+  <si>
+    <t>System shows password strength or length error
+Password meeting criteria accepted</t>
+  </si>
+  <si>
+    <t>System shows error indicating email already exists</t>
+  </si>
+  <si>
+    <t>Register button enabled only after mandatory fields are filled correctly</t>
+  </si>
+  <si>
+    <t>All validation/error messages are clear and user-friendly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	All fields, labels, buttons are visible, aligned, and readable</t>
+  </si>
+  <si>
+    <t>Registration works correctly on all browsers</t>
+  </si>
+  <si>
+    <t>Registration form is responsive and usable on mobile</t>
+  </si>
+  <si>
+    <t>Validation messages displayed</t>
+  </si>
+  <si>
+    <t>User registered Succesfully</t>
   </si>
 </sst>
 </file>
@@ -409,11 +399,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,43 +699,43 @@
     <col min="4" max="4" width="37.44140625" customWidth="1"/>
     <col min="5" max="5" width="36.88671875" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" customWidth="1"/>
-    <col min="7" max="7" width="72.5546875" customWidth="1"/>
+    <col min="7" max="7" width="53.88671875" customWidth="1"/>
     <col min="8" max="8" width="71.5546875" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -757,22 +747,22 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
@@ -787,25 +777,25 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>13</v>
@@ -817,28 +807,28 @@
     </row>
     <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>13</v>
@@ -850,28 +840,28 @@
     </row>
     <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>13</v>
@@ -883,263 +873,263 @@
     </row>
     <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>77</v>
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="4" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>40</v>
+        <v>85</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>67</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="K13" s="5"/>
     </row>

</xml_diff>